<commit_message>
Added m2 multiple runs and fixed some bugs
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\OneDrive\Documenten\BiBC\Major_internship\tcell-family-based\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238756DC-8DAD-4741-BD5C-0D79977FDE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38182498-6537-40EB-B087-6E3B483BA332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="0" windowWidth="26550" windowHeight="15585" xr2:uid="{D5E85D3C-A18F-46EA-BE25-41D4757F3CE4}"/>
+    <workbookView xWindow="105" yWindow="135" windowWidth="28800" windowHeight="15345" xr2:uid="{D5E85D3C-A18F-46EA-BE25-41D4757F3CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Parameters</t>
   </si>
@@ -182,9 +182,6 @@
     <t>0.15</t>
   </si>
   <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t>'sqrt(q*12.6)'</t>
   </si>
   <si>
@@ -192,13 +189,16 @@
   </si>
   <si>
     <t>rbeta(nr_of_families, shape1 = 2.29, shape2 = 3.80)'</t>
+  </si>
+  <si>
+    <t>2.5/0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,13 +214,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,10 +244,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -244,8 +257,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,7 +599,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,23 +648,29 @@
         <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -666,21 +690,27 @@
       <c r="E4" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -698,40 +728,49 @@
         <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>500</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>500</v>
       </c>
+      <c r="F7" s="4">
+        <v>500</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -749,40 +788,49 @@
         <v>46</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="b">
+      <c r="D10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -802,55 +850,67 @@
       <c r="E12" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F12" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="b">
+      <c r="D13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="F14" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -865,9 +925,12 @@
         <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>